<commit_message>
Age bias adjusted version 1
</commit_message>
<xml_diff>
--- a/data/Ages_sampled_v2.xlsx
+++ b/data/Ages_sampled_v2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Harpseals/HSmodel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{0F27ED7A-2D70-4AB2-828C-3BADD83120CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9056567E-A93C-4BE5-BC45-8E3C7D383F7D}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{0F27ED7A-2D70-4AB2-828C-3BADD83120CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FF731BA-58C8-4BBC-A294-6024898488C1}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="870" windowWidth="27015" windowHeight="15330" xr2:uid="{E3F39FE5-575D-42B4-891A-80E7B28E02A2}"/>
+    <workbookView xWindow="12405" yWindow="1380" windowWidth="32490" windowHeight="19245" xr2:uid="{E3F39FE5-575D-42B4-891A-80E7B28E02A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -113,6 +114,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5532A3-E30B-4F68-A6C3-0C38EC41E716}">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AY14" sqref="AY14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5162,4 +5167,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FF0C75-1B53-4646-88E2-0BF516BA9E1F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>